<commit_message>
Working on Supplemental Figures
</commit_message>
<xml_diff>
--- a/tables/file.inventory.xlsx
+++ b/tables/file.inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Box/Mito Transferome Unmixed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Documents/GitHub/mtD2/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E24C7C2-E92E-1144-B133-565881903441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE53CB9-4BA7-8145-8ED1-484DE81F2E16}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="2960" windowWidth="26040" windowHeight="14540" xr2:uid="{7D547BFD-3665-AD45-9074-16969955B0F5}"/>
   </bookViews>
@@ -186,9 +186,6 @@
     <t>file_id</t>
   </si>
   <si>
-    <t>patient_id</t>
-  </si>
-  <si>
     <t>sample_id</t>
   </si>
   <si>
@@ -355,6 +352,9 @@
   </si>
   <si>
     <t>age</t>
+  </si>
+  <si>
+    <t>tissue</t>
   </si>
 </sst>
 </file>
@@ -715,7 +715,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,13 +731,13 @@
         <v>50</v>
       </c>
       <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
         <v>51</v>
       </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -745,16 +745,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -762,16 +762,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -779,16 +779,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -796,16 +796,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -813,16 +813,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -830,16 +830,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -847,16 +847,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -864,16 +864,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -881,16 +881,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -898,16 +898,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -915,16 +915,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -932,16 +932,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -949,16 +949,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -966,16 +966,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -983,16 +983,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1000,16 +1000,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1017,16 +1017,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1034,16 +1034,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1051,16 +1051,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1068,16 +1068,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1085,16 +1085,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1102,16 +1102,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1119,16 +1119,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E24" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1136,16 +1136,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1153,16 +1153,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1170,16 +1170,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1187,16 +1187,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1204,16 +1204,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1221,16 +1221,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E30" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1238,16 +1238,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1255,16 +1255,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1272,16 +1272,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1289,16 +1289,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1306,16 +1306,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1323,16 +1323,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1340,16 +1340,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1357,16 +1357,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1374,16 +1374,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1391,16 +1391,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1408,16 +1408,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1425,16 +1425,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1442,16 +1442,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E43" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1459,16 +1459,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1476,16 +1476,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" t="s">
         <v>101</v>
       </c>
-      <c r="D45" t="s">
-        <v>102</v>
-      </c>
       <c r="E45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1493,16 +1493,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1510,16 +1510,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1527,16 +1527,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
         <v>101</v>
       </c>
-      <c r="D48" t="s">
-        <v>102</v>
-      </c>
       <c r="E48" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1544,16 +1544,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E49" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1561,16 +1561,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" t="s">
         <v>100</v>
       </c>
-      <c r="C50" t="s">
-        <v>101</v>
-      </c>
       <c r="D50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>